<commit_message>
Create mastermaster event detail page, modify some style
</commit_message>
<xml_diff>
--- a/Emergence_WPF/Document/Emergence项目API.xlsx
+++ b/Emergence_WPF/Document/Emergence项目API.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Emergence_Project\ElecSolution\Emergence_WPF\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="128">
   <si>
     <t>1. 主事件列表查询API</t>
   </si>
@@ -385,6 +385,42 @@
   </si>
   <si>
     <t>页面</t>
+  </si>
+  <si>
+    <t>数据里面的时间为创建时间，搜索的时间去掉。</t>
+  </si>
+  <si>
+    <t>归档去掉</t>
+  </si>
+  <si>
+    <t>物资都按个来算</t>
+  </si>
+  <si>
+    <t>地图标会跟子事件大页面地图相同</t>
+  </si>
+  <si>
+    <t>子事件详情</t>
+  </si>
+  <si>
+    <t>导入文本不需要</t>
+  </si>
+  <si>
+    <t>按照数据多的来做，队伍详情页面按照数据多的来。数据都是手动输入。</t>
+  </si>
+  <si>
+    <t>保存模版内容，如果是自己输入的，预设数据留空。</t>
+  </si>
+  <si>
+    <t>不做查询</t>
+  </si>
+  <si>
+    <t>不需要</t>
+  </si>
+  <si>
+    <t>按照最多的来</t>
+  </si>
+  <si>
+    <t>就按照现在的，保存模版内容，如果是自己输入的，预设数据留空。</t>
   </si>
 </sst>
 </file>
@@ -747,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,6 +878,9 @@
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -849,6 +888,9 @@
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,6 +984,9 @@
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,6 +1086,9 @@
       <c r="B33" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C33" t="s">
+        <v>119</v>
+      </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1097,6 +1145,9 @@
       </c>
       <c r="B40" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>120</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -1578,6 +1629,9 @@
       <c r="B102" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="C102" t="s">
+        <v>124</v>
+      </c>
       <c r="E102" s="5"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -1634,6 +1688,9 @@
       </c>
       <c r="B109" s="3" t="s">
         <v>94</v>
+      </c>
+      <c r="C109" t="s">
+        <v>125</v>
       </c>
       <c r="E109" s="5"/>
     </row>
@@ -1642,6 +1699,9 @@
       <c r="B110" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="C110" t="s">
+        <v>126</v>
+      </c>
       <c r="E110" s="5"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -1663,12 +1723,18 @@
       <c r="B113" t="s">
         <v>97</v>
       </c>
+      <c r="C113" t="s">
+        <v>121</v>
+      </c>
       <c r="E113" s="5"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>98</v>
       </c>
+      <c r="C114" t="s">
+        <v>122</v>
+      </c>
       <c r="E114" s="5"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,6 +1759,9 @@
       <c r="B118" t="s">
         <v>102</v>
       </c>
+      <c r="C118" t="s">
+        <v>123</v>
+      </c>
       <c r="E118" s="5"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -1773,6 +1842,9 @@
       </c>
       <c r="B129" s="3" t="s">
         <v>111</v>
+      </c>
+      <c r="C129" t="s">
+        <v>127</v>
       </c>
       <c r="E129" s="5"/>
     </row>

</xml_diff>

<commit_message>
Revert "Create mastermaster event detail page, modify some style"
This reverts commit 65ab133b97dd9cda228c9a5712d7fdbb1c0fe8e7.
</commit_message>
<xml_diff>
--- a/Emergence_WPF/Document/Emergence项目API.xlsx
+++ b/Emergence_WPF/Document/Emergence项目API.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Emergence_Project\ElecSolution\Emergence_WPF\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="116">
   <si>
     <t>1. 主事件列表查询API</t>
   </si>
@@ -385,42 +385,6 @@
   </si>
   <si>
     <t>页面</t>
-  </si>
-  <si>
-    <t>数据里面的时间为创建时间，搜索的时间去掉。</t>
-  </si>
-  <si>
-    <t>归档去掉</t>
-  </si>
-  <si>
-    <t>物资都按个来算</t>
-  </si>
-  <si>
-    <t>地图标会跟子事件大页面地图相同</t>
-  </si>
-  <si>
-    <t>子事件详情</t>
-  </si>
-  <si>
-    <t>导入文本不需要</t>
-  </si>
-  <si>
-    <t>按照数据多的来做，队伍详情页面按照数据多的来。数据都是手动输入。</t>
-  </si>
-  <si>
-    <t>保存模版内容，如果是自己输入的，预设数据留空。</t>
-  </si>
-  <si>
-    <t>不做查询</t>
-  </si>
-  <si>
-    <t>不需要</t>
-  </si>
-  <si>
-    <t>按照最多的来</t>
-  </si>
-  <si>
-    <t>就按照现在的，保存模版内容，如果是自己输入的，预设数据留空。</t>
   </si>
 </sst>
 </file>
@@ -783,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,9 +842,6 @@
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>116</v>
-      </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -888,9 +849,6 @@
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>117</v>
-      </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -984,9 +942,6 @@
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>118</v>
-      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1086,9 +1041,6 @@
       <c r="B33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C33" t="s">
-        <v>119</v>
-      </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1145,9 +1097,6 @@
       </c>
       <c r="B40" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -1629,9 +1578,6 @@
       <c r="B102" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C102" t="s">
-        <v>124</v>
-      </c>
       <c r="E102" s="5"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,9 +1634,6 @@
       </c>
       <c r="B109" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C109" t="s">
-        <v>125</v>
       </c>
       <c r="E109" s="5"/>
     </row>
@@ -1699,9 +1642,6 @@
       <c r="B110" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C110" t="s">
-        <v>126</v>
-      </c>
       <c r="E110" s="5"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,18 +1663,12 @@
       <c r="B113" t="s">
         <v>97</v>
       </c>
-      <c r="C113" t="s">
-        <v>121</v>
-      </c>
       <c r="E113" s="5"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>98</v>
       </c>
-      <c r="C114" t="s">
-        <v>122</v>
-      </c>
       <c r="E114" s="5"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -1759,9 +1693,6 @@
       <c r="B118" t="s">
         <v>102</v>
       </c>
-      <c r="C118" t="s">
-        <v>123</v>
-      </c>
       <c r="E118" s="5"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -1842,9 +1773,6 @@
       </c>
       <c r="B129" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="C129" t="s">
-        <v>127</v>
       </c>
       <c r="E129" s="5"/>
     </row>

</xml_diff>